<commit_message>
Updated sprint backblog, product backlog and user stories
</commit_message>
<xml_diff>
--- a/Project Backlog/User Stories.xlsx
+++ b/Project Backlog/User Stories.xlsx
@@ -4,14 +4,43 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Copy of Sheet1" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="E24">
+      <text>
+        <t xml:space="preserve">Is anything additional needed here?
+	-Kayla Wallace</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="B6">
+      <text>
+        <t xml:space="preserve">Is this so that a player can choose a colour OR an icon or can they choose both?
+	-Kayla Wallace</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="E8">
+      <text>
+        <t xml:space="preserve">Ask back end team how we will ensure questions are not repeated
+	-Kayla Wallace</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="64">
   <si>
     <t>USER STORIES</t>
   </si>
@@ -37,57 +66,112 @@
     <t>As a player, I can play a single-player game.</t>
   </si>
   <si>
+    <t>n/a</t>
+  </si>
+  <si>
     <t>As a player, I can input a custom nickname.</t>
   </si>
   <si>
+    <t>- Player will be able to type their chosen nickname into a text input box before the game begins
+- Length to be between 1 and 30 characters</t>
+  </si>
+  <si>
     <t>As a player, I can select a player icon from a given selection.</t>
   </si>
   <si>
+    <t>- A selection of at least 3 icons to be displayed to the player
+- The player will be given a default if they do not choose an icon
+- If an icon is chosen, the icon will be assigned to the player for the current game only</t>
+  </si>
+  <si>
     <t>As a player, I can select a player colour to uniquely identify myself.</t>
   </si>
   <si>
     <t xml:space="preserve">As a player, I can select an answer to input from the four answers given with the question. </t>
   </si>
   <si>
+    <t>- Four answer choices will be displayed to the user
+- Player can only choose one answer</t>
+  </si>
+  <si>
     <t>As a player, I want to receive random questions so we cannot get asked the same question multiple times in a quiz, or in quick succession of quizzes.</t>
   </si>
   <si>
+    <t>- Questions will be fetched from the database randomly</t>
+  </si>
+  <si>
     <t xml:space="preserve">As a player, I can see my score update based on my answer. </t>
   </si>
   <si>
+    <t>- Scores for all players will be displayed on the leaderboard throughout the game</t>
+  </si>
+  <si>
     <t xml:space="preserve">As a player, I can recieve more points based on quickly I enter a correct answer. </t>
   </si>
   <si>
+    <t>- An algorithm will be determined by the team such that the points awarded to the players will be according to the time taken to answer the question (faster = more points)
+- If the players do not answer the question within the time limit or get the question wrong, no points will be given to them</t>
+  </si>
+  <si>
     <t>As a player, I can exit a game at any time.</t>
   </si>
   <si>
     <t xml:space="preserve">As a player, I can play the game on a browser of my choosing. </t>
   </si>
   <si>
+    <t>- Google Chrome, Firefox, Microsoft Edge, Internet Explorer, Safari</t>
+  </si>
+  <si>
     <t>As a player, I can join a multiplayer game.</t>
   </si>
   <si>
+    <t xml:space="preserve">- Up to 10 people in a single game </t>
+  </si>
+  <si>
     <t>As a player, I have a time limit to answer each question.</t>
   </si>
   <si>
+    <t>- Initially, the time limit will be fixed to 30 seconds.
+- If time, the team would like to implement a feature allowing the player to choose the time limit, ranging from 10 seconds to 1 minute.</t>
+  </si>
+  <si>
     <t>As a player, I want to share my screen name with the other players as this will help with immersion and help me identify who I am playing against.</t>
   </si>
   <si>
+    <t>- Player nicknames will be displayed in the leaderboard on the screen to all players in the game
+- The team hopes to implement a chat function, player nicknames will be displayed to all players in the game beside any messages sent by them</t>
+  </si>
+  <si>
     <t>As a player, I want to join a game only using a code given to me by my friend, as this will prevent joining the wrong game.</t>
   </si>
   <si>
+    <t>- Unique code to be generated and sent to the game host who can give this to their friends to allow them to play in a private game together</t>
+  </si>
+  <si>
     <t xml:space="preserve">As a player, if I get below a certain points level, I should be eliminated from the round. </t>
   </si>
   <si>
+    <t>- A point threshold will be assigned in each round
+- If a player's points go below the threshold, then they will be eliminated from the game</t>
+  </si>
+  <si>
     <t>As a player, I want to be able to see a real time scoring leaderboard to see who is winning the game and where I place in relation to the rest of the players.</t>
   </si>
   <si>
+    <t>- Leaderboard will be visible on the screen during all rounds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a player, I should recieve trophy badges based on my actions in the game.                     </t>
+  </si>
+  <si>
+    <t>- Badges will be displayed next to players names throughout the game
+- Badges can change who they are assigned to throughout the game
+- Will include: fastest, slowest, most accurate.</t>
+  </si>
+  <si>
     <t>As a player, I should recieve special items for getting random answers correct.</t>
   </si>
   <si>
-    <t xml:space="preserve">As a player, I should recieve trophy badges based on my actions in the game.                     </t>
-  </si>
-  <si>
     <t>As a player, I should be able to use items to affect my score or other players score/answers, as a fun "saboutage" add-on the game.</t>
   </si>
   <si>
@@ -97,10 +181,11 @@
     <t>As a game host, I can create a lobby so that I can play with friends.</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a game host, I can create a unique game code so I can share it with my friends so only they can play with me.
+    <t xml:space="preserve">- Lobby will allow up to 10 people for a game
+- Other players can access the lobby using the code generated and given to the game host </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a game host, I can receive a unique game code so I can share it with my friends so only they can play with me.
 </t>
   </si>
   <si>
@@ -110,35 +195,202 @@
     <t>As a developer, I want to ensure the colour contrast in the game meets WCAG guidelines.</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <rFont val="Century Gothic"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve">"Success Criterion </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Century Gothic"/>
+        <color rgb="FF000000"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>1.4.3 Contrast (Minimum)</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Century Gothic"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve"> (Level AA): The visual presentation of </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Century Gothic"/>
+        <color rgb="FF000000"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>text</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Century Gothic"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Century Gothic"/>
+        <color rgb="FF000000"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>images of text</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Century Gothic"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve"> has a </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Century Gothic"/>
+        <color rgb="FF000000"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>contrast ratio</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Century Gothic"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve"> of at least 4.5:1" - WCAG</t>
+    </r>
+  </si>
+  <si>
+    <t>- Run the application through a colour contrast checker</t>
+  </si>
+  <si>
     <t xml:space="preserve">As a developer, I want to ensure the font size meets the WCAG guidelines. </t>
   </si>
   <si>
+    <t>"Ensure that default fonts are no smaller than 9 pt (=12px). Smaller sizes may be illegible on some platforms. The WCAG Guidelines recommend ensuring that text can be zoomed to 200%."</t>
+  </si>
+  <si>
     <t>As a developer, I want to implement a scoring system based on the time taken to answer a question.</t>
   </si>
   <si>
+    <t>- The faster a player answers, the more points they will recieve. 
+- If they do not answer within the time limit or their answer is wrong, they will recieve no points for that question.</t>
+  </si>
+  <si>
     <t>As a developer, I want to create a database and publish on a server so I can store all the questions and answers to the quiz so they can be easily obtained</t>
   </si>
   <si>
+    <t xml:space="preserve">- Microsoft Azure will be used to host the server.
+- MDB will be used for database creation.
+- Data set will be converted to JSON format to be read and used.
+</t>
+  </si>
+  <si>
     <t>As a developer, I want a dataset with multiple choice questions so we do not have to format how answers are read into the system and prevent technically correct answers deemed as wrong</t>
   </si>
   <si>
+    <t>- Test to see if each question has 4 possible anwers associated with it.
+- Test if the true answer correctly updates the player's scores.</t>
+  </si>
+  <si>
     <t>As a developer, I want to be able to connect our web-app to our database in order to send questions to our players</t>
   </si>
   <si>
+    <t>- Use sockets to connect to the server, then split into different lobbies via their room code.
+- Use a direct connection to the database.</t>
+  </si>
+  <si>
     <t>As a developer, I want to be able to store the lobby using the unique game code in a seperate database, so I can have a unique identifier for each game currently being played.</t>
   </si>
   <si>
     <t>As a developer, I want to be able to update the player score after each round, so that the database can store the up to date scores for when the information is needed.</t>
   </si>
   <si>
+    <t>- Stored within Lobby DB
+- Team to work out algorithm for calculating scores
+- Team to work out what units to use, i.e 100’s, 1000’s, 10’s etc.</t>
+  </si>
+  <si>
     <t>As a developer, I want to be able to send the data from the database to the screen in a JSON format, as this will be a lightweight and appropriate data structure to use for the React based frontend.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Century Gothic"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve">"Success Criterion </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Century Gothic"/>
+        <color rgb="FF000000"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>1.4.3 Contrast (Minimum)</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Century Gothic"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve"> (Level AA): The visual presentation of </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Century Gothic"/>
+        <color rgb="FF000000"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>text</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Century Gothic"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Century Gothic"/>
+        <color rgb="FF000000"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>images of text</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Century Gothic"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve"> has a </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Century Gothic"/>
+        <color rgb="FF000000"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>contrast ratio</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Century Gothic"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve"> of at least 4.5:1" - WCAG</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -164,8 +416,18 @@
       <color rgb="FF000000"/>
       <name val="Century Gothic"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Sans-serif"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <color rgb="FF222222"/>
+      <name val="Century Gothic"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,6 +440,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -185,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -206,6 +474,15 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -215,6 +492,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -491,7 +772,9 @@
       <c r="D3" s="5">
         <v>8.0</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -510,7 +793,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="5">
         <v>9.0</v>
@@ -518,7 +801,9 @@
       <c r="D4" s="5">
         <v>6.0</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -537,7 +822,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C5" s="5">
         <v>9.0</v>
@@ -545,7 +830,9 @@
       <c r="D5" s="5">
         <v>6.0</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -564,7 +851,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C6" s="5">
         <v>9.0</v>
@@ -591,7 +878,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C7" s="5">
         <v>10.0</v>
@@ -599,7 +886,9 @@
       <c r="D7" s="5">
         <v>7.0</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -618,7 +907,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C8" s="5">
         <v>8.0</v>
@@ -626,7 +915,9 @@
       <c r="D8" s="5">
         <v>5.0</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -645,15 +936,17 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C9" s="5">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="D9" s="5">
         <v>6.0</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -672,7 +965,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C10" s="5">
         <v>10.0</v>
@@ -680,7 +973,9 @@
       <c r="D10" s="5">
         <v>7.0</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -699,7 +994,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C11" s="5">
         <v>10.0</v>
@@ -707,7 +1002,9 @@
       <c r="D11" s="5">
         <v>4.0</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -726,7 +1023,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C12" s="5">
         <v>8.0</v>
@@ -734,7 +1031,9 @@
       <c r="D12" s="5">
         <v>7.0</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -753,7 +1052,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C13" s="5">
         <v>9.0</v>
@@ -761,7 +1060,9 @@
       <c r="D13" s="5">
         <v>9.0</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -780,7 +1081,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C14" s="5">
         <v>8.0</v>
@@ -788,7 +1089,9 @@
       <c r="D14" s="5">
         <v>5.0</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -807,7 +1110,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C15" s="5">
         <v>9.0</v>
@@ -815,7 +1118,9 @@
       <c r="D15" s="5">
         <v>9.0</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -834,7 +1139,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C16" s="5">
         <v>9.0</v>
@@ -842,7 +1147,9 @@
       <c r="D16" s="5">
         <v>9.0</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -861,7 +1168,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C17" s="5">
         <v>2.0</v>
@@ -869,7 +1176,9 @@
       <c r="D17" s="5">
         <v>7.0</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -893,7 +1202,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C18" s="5">
         <v>8.0</v>
@@ -901,7 +1210,9 @@
       <c r="D18" s="5">
         <v>8.0</v>
       </c>
-      <c r="E18" s="2"/>
+      <c r="E18" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -920,15 +1231,17 @@
         <v>17</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C19" s="5">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="D19" s="5">
         <v>7.0</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -952,10 +1265,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C20" s="5">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="D20" s="5">
         <v>7.0</v>
@@ -984,7 +1297,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C21" s="5">
         <v>2.0</v>
@@ -1016,7 +1329,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C22" s="5">
         <v>3.0</v>
@@ -1048,7 +1361,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="C23" s="5">
         <v>10.0</v>
@@ -1056,8 +1369,8 @@
       <c r="D23" s="5">
         <v>9.0</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>28</v>
+      <c r="E23" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1082,7 +1395,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C24" s="5">
         <v>9.0</v>
@@ -1090,7 +1403,9 @@
       <c r="D24" s="5">
         <v>9.0</v>
       </c>
-      <c r="E24" s="2"/>
+      <c r="E24" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -1114,7 +1429,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C25" s="5">
         <v>3.0</v>
@@ -1122,7 +1437,9 @@
       <c r="D25" s="5">
         <v>9.0</v>
       </c>
-      <c r="E25" s="2"/>
+      <c r="E25" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -1141,7 +1458,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C26" s="5">
         <v>6.0</v>
@@ -1149,8 +1466,12 @@
       <c r="D26" s="5">
         <v>4.0</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="E26" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -1168,7 +1489,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C27" s="5">
         <v>6.0</v>
@@ -1176,7 +1497,9 @@
       <c r="D27" s="5">
         <v>3.0</v>
       </c>
-      <c r="E27" s="2"/>
+      <c r="E27" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -1195,7 +1518,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C28" s="5">
         <v>8.0</v>
@@ -1203,7 +1526,9 @@
       <c r="D28" s="5">
         <v>7.0</v>
       </c>
-      <c r="E28" s="2"/>
+      <c r="E28" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -1222,7 +1547,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="C29" s="5">
         <v>10.0</v>
@@ -1230,7 +1555,9 @@
       <c r="D29" s="5">
         <v>6.0</v>
       </c>
-      <c r="E29" s="2"/>
+      <c r="E29" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -1254,7 +1581,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="C30" s="5">
         <v>8.0</v>
@@ -1262,8 +1589,12 @@
       <c r="D30" s="5">
         <v>6.0</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="E30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -1286,7 +1617,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C31" s="5">
         <v>10.0</v>
@@ -1294,7 +1625,9 @@
       <c r="D31" s="5">
         <v>7.0</v>
       </c>
-      <c r="E31" s="2"/>
+      <c r="E31" s="6" t="s">
+        <v>58</v>
+      </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -1318,7 +1651,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="C32" s="5">
         <v>9.0</v>
@@ -1326,7 +1659,9 @@
       <c r="D32" s="5">
         <v>10.0</v>
       </c>
-      <c r="E32" s="2"/>
+      <c r="E32" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -1350,7 +1685,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="C33" s="5">
         <v>3.0</v>
@@ -1358,7 +1693,9 @@
       <c r="D33" s="5">
         <v>9.0</v>
       </c>
-      <c r="E33" s="2"/>
+      <c r="E33" s="7" t="s">
+        <v>61</v>
+      </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -1382,7 +1719,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="C34" s="5">
         <v>10.0</v>
@@ -1390,7 +1727,9 @@
       <c r="D34" s="5">
         <v>7.0</v>
       </c>
-      <c r="E34" s="2"/>
+      <c r="E34" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -2827,6 +3166,2490 @@
       <c r="U95" s="2"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId2" location="dfn-contrast-ratio" ref="E26"/>
+  </hyperlinks>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="85.43"/>
+    <col customWidth="1" min="5" max="5" width="23.86"/>
+    <col customWidth="1" min="6" max="6" width="17.86"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="24.75" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <f t="shared" ref="A3:A39" si="1">ROW()-2</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="D13" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="D14" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="D15" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="D16" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D17" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="D18" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="D19" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D20" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D21" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="D22" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="D23" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+    </row>
+    <row r="24" ht="31.5" customHeight="1">
+      <c r="A24" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="D24" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="D25" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="D26" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="D27" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="D28" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="D29" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="D30" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="D31" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="D32" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="D33" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="D34" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="2"/>
+      <c r="S41" s="2"/>
+      <c r="T41" s="2"/>
+      <c r="U41" s="2"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="2"/>
+      <c r="S42" s="2"/>
+      <c r="T42" s="2"/>
+      <c r="U42" s="2"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+      <c r="U43" s="2"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="2"/>
+      <c r="S44" s="2"/>
+      <c r="T44" s="2"/>
+      <c r="U44" s="2"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+      <c r="R45" s="2"/>
+      <c r="S45" s="2"/>
+      <c r="T45" s="2"/>
+      <c r="U45" s="2"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+      <c r="R46" s="2"/>
+      <c r="S46" s="2"/>
+      <c r="T46" s="2"/>
+      <c r="U46" s="2"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="2"/>
+      <c r="S47" s="2"/>
+      <c r="T47" s="2"/>
+      <c r="U47" s="2"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+      <c r="R48" s="2"/>
+      <c r="S48" s="2"/>
+      <c r="T48" s="2"/>
+      <c r="U48" s="2"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
+      <c r="R49" s="2"/>
+      <c r="S49" s="2"/>
+      <c r="T49" s="2"/>
+      <c r="U49" s="2"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2"/>
+      <c r="S50" s="2"/>
+      <c r="T50" s="2"/>
+      <c r="U50" s="2"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2"/>
+      <c r="R51" s="2"/>
+      <c r="S51" s="2"/>
+      <c r="T51" s="2"/>
+      <c r="U51" s="2"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="2"/>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="2"/>
+      <c r="S52" s="2"/>
+      <c r="T52" s="2"/>
+      <c r="U52" s="2"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+      <c r="P53" s="2"/>
+      <c r="Q53" s="2"/>
+      <c r="R53" s="2"/>
+      <c r="S53" s="2"/>
+      <c r="T53" s="2"/>
+      <c r="U53" s="2"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+      <c r="O54" s="2"/>
+      <c r="P54" s="2"/>
+      <c r="Q54" s="2"/>
+      <c r="R54" s="2"/>
+      <c r="S54" s="2"/>
+      <c r="T54" s="2"/>
+      <c r="U54" s="2"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
+      <c r="P55" s="2"/>
+      <c r="Q55" s="2"/>
+      <c r="R55" s="2"/>
+      <c r="S55" s="2"/>
+      <c r="T55" s="2"/>
+      <c r="U55" s="2"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
+      <c r="O56" s="2"/>
+      <c r="P56" s="2"/>
+      <c r="Q56" s="2"/>
+      <c r="R56" s="2"/>
+      <c r="S56" s="2"/>
+      <c r="T56" s="2"/>
+      <c r="U56" s="2"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
+      <c r="O57" s="2"/>
+      <c r="P57" s="2"/>
+      <c r="Q57" s="2"/>
+      <c r="R57" s="2"/>
+      <c r="S57" s="2"/>
+      <c r="T57" s="2"/>
+      <c r="U57" s="2"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
+      <c r="O58" s="2"/>
+      <c r="P58" s="2"/>
+      <c r="Q58" s="2"/>
+      <c r="R58" s="2"/>
+      <c r="S58" s="2"/>
+      <c r="T58" s="2"/>
+      <c r="U58" s="2"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
+      <c r="O59" s="2"/>
+      <c r="P59" s="2"/>
+      <c r="Q59" s="2"/>
+      <c r="R59" s="2"/>
+      <c r="S59" s="2"/>
+      <c r="T59" s="2"/>
+      <c r="U59" s="2"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
+      <c r="O60" s="2"/>
+      <c r="P60" s="2"/>
+      <c r="Q60" s="2"/>
+      <c r="R60" s="2"/>
+      <c r="S60" s="2"/>
+      <c r="T60" s="2"/>
+      <c r="U60" s="2"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="2"/>
+      <c r="N61" s="2"/>
+      <c r="O61" s="2"/>
+      <c r="P61" s="2"/>
+      <c r="Q61" s="2"/>
+      <c r="R61" s="2"/>
+      <c r="S61" s="2"/>
+      <c r="T61" s="2"/>
+      <c r="U61" s="2"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
+      <c r="O62" s="2"/>
+      <c r="P62" s="2"/>
+      <c r="Q62" s="2"/>
+      <c r="R62" s="2"/>
+      <c r="S62" s="2"/>
+      <c r="T62" s="2"/>
+      <c r="U62" s="2"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+      <c r="M63" s="2"/>
+      <c r="N63" s="2"/>
+      <c r="O63" s="2"/>
+      <c r="P63" s="2"/>
+      <c r="Q63" s="2"/>
+      <c r="R63" s="2"/>
+      <c r="S63" s="2"/>
+      <c r="T63" s="2"/>
+      <c r="U63" s="2"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+      <c r="M64" s="2"/>
+      <c r="N64" s="2"/>
+      <c r="O64" s="2"/>
+      <c r="P64" s="2"/>
+      <c r="Q64" s="2"/>
+      <c r="R64" s="2"/>
+      <c r="S64" s="2"/>
+      <c r="T64" s="2"/>
+      <c r="U64" s="2"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+      <c r="M65" s="2"/>
+      <c r="N65" s="2"/>
+      <c r="O65" s="2"/>
+      <c r="P65" s="2"/>
+      <c r="Q65" s="2"/>
+      <c r="R65" s="2"/>
+      <c r="S65" s="2"/>
+      <c r="T65" s="2"/>
+      <c r="U65" s="2"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+      <c r="M66" s="2"/>
+      <c r="N66" s="2"/>
+      <c r="O66" s="2"/>
+      <c r="P66" s="2"/>
+      <c r="Q66" s="2"/>
+      <c r="R66" s="2"/>
+      <c r="S66" s="2"/>
+      <c r="T66" s="2"/>
+      <c r="U66" s="2"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+      <c r="L67" s="2"/>
+      <c r="M67" s="2"/>
+      <c r="N67" s="2"/>
+      <c r="O67" s="2"/>
+      <c r="P67" s="2"/>
+      <c r="Q67" s="2"/>
+      <c r="R67" s="2"/>
+      <c r="S67" s="2"/>
+      <c r="T67" s="2"/>
+      <c r="U67" s="2"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+      <c r="M68" s="2"/>
+      <c r="N68" s="2"/>
+      <c r="O68" s="2"/>
+      <c r="P68" s="2"/>
+      <c r="Q68" s="2"/>
+      <c r="R68" s="2"/>
+      <c r="S68" s="2"/>
+      <c r="T68" s="2"/>
+      <c r="U68" s="2"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+      <c r="M69" s="2"/>
+      <c r="N69" s="2"/>
+      <c r="O69" s="2"/>
+      <c r="P69" s="2"/>
+      <c r="Q69" s="2"/>
+      <c r="R69" s="2"/>
+      <c r="S69" s="2"/>
+      <c r="T69" s="2"/>
+      <c r="U69" s="2"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+      <c r="K70" s="2"/>
+      <c r="L70" s="2"/>
+      <c r="M70" s="2"/>
+      <c r="N70" s="2"/>
+      <c r="O70" s="2"/>
+      <c r="P70" s="2"/>
+      <c r="Q70" s="2"/>
+      <c r="R70" s="2"/>
+      <c r="S70" s="2"/>
+      <c r="T70" s="2"/>
+      <c r="U70" s="2"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2"/>
+      <c r="K71" s="2"/>
+      <c r="L71" s="2"/>
+      <c r="M71" s="2"/>
+      <c r="N71" s="2"/>
+      <c r="O71" s="2"/>
+      <c r="P71" s="2"/>
+      <c r="Q71" s="2"/>
+      <c r="R71" s="2"/>
+      <c r="S71" s="2"/>
+      <c r="T71" s="2"/>
+      <c r="U71" s="2"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2"/>
+      <c r="K72" s="2"/>
+      <c r="L72" s="2"/>
+      <c r="M72" s="2"/>
+      <c r="N72" s="2"/>
+      <c r="O72" s="2"/>
+      <c r="P72" s="2"/>
+      <c r="Q72" s="2"/>
+      <c r="R72" s="2"/>
+      <c r="S72" s="2"/>
+      <c r="T72" s="2"/>
+      <c r="U72" s="2"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+      <c r="K73" s="2"/>
+      <c r="L73" s="2"/>
+      <c r="M73" s="2"/>
+      <c r="N73" s="2"/>
+      <c r="O73" s="2"/>
+      <c r="P73" s="2"/>
+      <c r="Q73" s="2"/>
+      <c r="R73" s="2"/>
+      <c r="S73" s="2"/>
+      <c r="T73" s="2"/>
+      <c r="U73" s="2"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
+      <c r="K74" s="2"/>
+      <c r="L74" s="2"/>
+      <c r="M74" s="2"/>
+      <c r="N74" s="2"/>
+      <c r="O74" s="2"/>
+      <c r="P74" s="2"/>
+      <c r="Q74" s="2"/>
+      <c r="R74" s="2"/>
+      <c r="S74" s="2"/>
+      <c r="T74" s="2"/>
+      <c r="U74" s="2"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
+      <c r="I75" s="2"/>
+      <c r="J75" s="2"/>
+      <c r="K75" s="2"/>
+      <c r="L75" s="2"/>
+      <c r="M75" s="2"/>
+      <c r="N75" s="2"/>
+      <c r="O75" s="2"/>
+      <c r="P75" s="2"/>
+      <c r="Q75" s="2"/>
+      <c r="R75" s="2"/>
+      <c r="S75" s="2"/>
+      <c r="T75" s="2"/>
+      <c r="U75" s="2"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="2"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2"/>
+      <c r="K76" s="2"/>
+      <c r="L76" s="2"/>
+      <c r="M76" s="2"/>
+      <c r="N76" s="2"/>
+      <c r="O76" s="2"/>
+      <c r="P76" s="2"/>
+      <c r="Q76" s="2"/>
+      <c r="R76" s="2"/>
+      <c r="S76" s="2"/>
+      <c r="T76" s="2"/>
+      <c r="U76" s="2"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="2"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
+      <c r="J77" s="2"/>
+      <c r="K77" s="2"/>
+      <c r="L77" s="2"/>
+      <c r="M77" s="2"/>
+      <c r="N77" s="2"/>
+      <c r="O77" s="2"/>
+      <c r="P77" s="2"/>
+      <c r="Q77" s="2"/>
+      <c r="R77" s="2"/>
+      <c r="S77" s="2"/>
+      <c r="T77" s="2"/>
+      <c r="U77" s="2"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="2"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
+      <c r="J78" s="2"/>
+      <c r="K78" s="2"/>
+      <c r="L78" s="2"/>
+      <c r="M78" s="2"/>
+      <c r="N78" s="2"/>
+      <c r="O78" s="2"/>
+      <c r="P78" s="2"/>
+      <c r="Q78" s="2"/>
+      <c r="R78" s="2"/>
+      <c r="S78" s="2"/>
+      <c r="T78" s="2"/>
+      <c r="U78" s="2"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="2"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
+      <c r="H79" s="2"/>
+      <c r="I79" s="2"/>
+      <c r="J79" s="2"/>
+      <c r="K79" s="2"/>
+      <c r="L79" s="2"/>
+      <c r="M79" s="2"/>
+      <c r="N79" s="2"/>
+      <c r="O79" s="2"/>
+      <c r="P79" s="2"/>
+      <c r="Q79" s="2"/>
+      <c r="R79" s="2"/>
+      <c r="S79" s="2"/>
+      <c r="T79" s="2"/>
+      <c r="U79" s="2"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+      <c r="J80" s="2"/>
+      <c r="K80" s="2"/>
+      <c r="L80" s="2"/>
+      <c r="M80" s="2"/>
+      <c r="N80" s="2"/>
+      <c r="O80" s="2"/>
+      <c r="P80" s="2"/>
+      <c r="Q80" s="2"/>
+      <c r="R80" s="2"/>
+      <c r="S80" s="2"/>
+      <c r="T80" s="2"/>
+      <c r="U80" s="2"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
+      <c r="J81" s="2"/>
+      <c r="K81" s="2"/>
+      <c r="L81" s="2"/>
+      <c r="M81" s="2"/>
+      <c r="N81" s="2"/>
+      <c r="O81" s="2"/>
+      <c r="P81" s="2"/>
+      <c r="Q81" s="2"/>
+      <c r="R81" s="2"/>
+      <c r="S81" s="2"/>
+      <c r="T81" s="2"/>
+      <c r="U81" s="2"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="2"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+      <c r="I82" s="2"/>
+      <c r="J82" s="2"/>
+      <c r="K82" s="2"/>
+      <c r="L82" s="2"/>
+      <c r="M82" s="2"/>
+      <c r="N82" s="2"/>
+      <c r="O82" s="2"/>
+      <c r="P82" s="2"/>
+      <c r="Q82" s="2"/>
+      <c r="R82" s="2"/>
+      <c r="S82" s="2"/>
+      <c r="T82" s="2"/>
+      <c r="U82" s="2"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="2"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2"/>
+      <c r="I83" s="2"/>
+      <c r="J83" s="2"/>
+      <c r="K83" s="2"/>
+      <c r="L83" s="2"/>
+      <c r="M83" s="2"/>
+      <c r="N83" s="2"/>
+      <c r="O83" s="2"/>
+      <c r="P83" s="2"/>
+      <c r="Q83" s="2"/>
+      <c r="R83" s="2"/>
+      <c r="S83" s="2"/>
+      <c r="T83" s="2"/>
+      <c r="U83" s="2"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="2"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
+      <c r="H84" s="2"/>
+      <c r="I84" s="2"/>
+      <c r="J84" s="2"/>
+      <c r="K84" s="2"/>
+      <c r="L84" s="2"/>
+      <c r="M84" s="2"/>
+      <c r="N84" s="2"/>
+      <c r="O84" s="2"/>
+      <c r="P84" s="2"/>
+      <c r="Q84" s="2"/>
+      <c r="R84" s="2"/>
+      <c r="S84" s="2"/>
+      <c r="T84" s="2"/>
+      <c r="U84" s="2"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="2"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
+      <c r="J85" s="2"/>
+      <c r="K85" s="2"/>
+      <c r="L85" s="2"/>
+      <c r="M85" s="2"/>
+      <c r="N85" s="2"/>
+      <c r="O85" s="2"/>
+      <c r="P85" s="2"/>
+      <c r="Q85" s="2"/>
+      <c r="R85" s="2"/>
+      <c r="S85" s="2"/>
+      <c r="T85" s="2"/>
+      <c r="U85" s="2"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="2"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="2"/>
+      <c r="I86" s="2"/>
+      <c r="J86" s="2"/>
+      <c r="K86" s="2"/>
+      <c r="L86" s="2"/>
+      <c r="M86" s="2"/>
+      <c r="N86" s="2"/>
+      <c r="O86" s="2"/>
+      <c r="P86" s="2"/>
+      <c r="Q86" s="2"/>
+      <c r="R86" s="2"/>
+      <c r="S86" s="2"/>
+      <c r="T86" s="2"/>
+      <c r="U86" s="2"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="2"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
+      <c r="J87" s="2"/>
+      <c r="K87" s="2"/>
+      <c r="L87" s="2"/>
+      <c r="M87" s="2"/>
+      <c r="N87" s="2"/>
+      <c r="O87" s="2"/>
+      <c r="P87" s="2"/>
+      <c r="Q87" s="2"/>
+      <c r="R87" s="2"/>
+      <c r="S87" s="2"/>
+      <c r="T87" s="2"/>
+      <c r="U87" s="2"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="2"/>
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="2"/>
+      <c r="H88" s="2"/>
+      <c r="I88" s="2"/>
+      <c r="J88" s="2"/>
+      <c r="K88" s="2"/>
+      <c r="L88" s="2"/>
+      <c r="M88" s="2"/>
+      <c r="N88" s="2"/>
+      <c r="O88" s="2"/>
+      <c r="P88" s="2"/>
+      <c r="Q88" s="2"/>
+      <c r="R88" s="2"/>
+      <c r="S88" s="2"/>
+      <c r="T88" s="2"/>
+      <c r="U88" s="2"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="2"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
+      <c r="H89" s="2"/>
+      <c r="I89" s="2"/>
+      <c r="J89" s="2"/>
+      <c r="K89" s="2"/>
+      <c r="L89" s="2"/>
+      <c r="M89" s="2"/>
+      <c r="N89" s="2"/>
+      <c r="O89" s="2"/>
+      <c r="P89" s="2"/>
+      <c r="Q89" s="2"/>
+      <c r="R89" s="2"/>
+      <c r="S89" s="2"/>
+      <c r="T89" s="2"/>
+      <c r="U89" s="2"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="2"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="2"/>
+      <c r="H90" s="2"/>
+      <c r="I90" s="2"/>
+      <c r="J90" s="2"/>
+      <c r="K90" s="2"/>
+      <c r="L90" s="2"/>
+      <c r="M90" s="2"/>
+      <c r="N90" s="2"/>
+      <c r="O90" s="2"/>
+      <c r="P90" s="2"/>
+      <c r="Q90" s="2"/>
+      <c r="R90" s="2"/>
+      <c r="S90" s="2"/>
+      <c r="T90" s="2"/>
+      <c r="U90" s="2"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="2"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="2"/>
+      <c r="H91" s="2"/>
+      <c r="I91" s="2"/>
+      <c r="J91" s="2"/>
+      <c r="K91" s="2"/>
+      <c r="L91" s="2"/>
+      <c r="M91" s="2"/>
+      <c r="N91" s="2"/>
+      <c r="O91" s="2"/>
+      <c r="P91" s="2"/>
+      <c r="Q91" s="2"/>
+      <c r="R91" s="2"/>
+      <c r="S91" s="2"/>
+      <c r="T91" s="2"/>
+      <c r="U91" s="2"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="2"/>
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="2"/>
+      <c r="K92" s="2"/>
+      <c r="L92" s="2"/>
+      <c r="M92" s="2"/>
+      <c r="N92" s="2"/>
+      <c r="O92" s="2"/>
+      <c r="P92" s="2"/>
+      <c r="Q92" s="2"/>
+      <c r="R92" s="2"/>
+      <c r="S92" s="2"/>
+      <c r="T92" s="2"/>
+      <c r="U92" s="2"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="2"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="2"/>
+      <c r="H93" s="2"/>
+      <c r="I93" s="2"/>
+      <c r="J93" s="2"/>
+      <c r="K93" s="2"/>
+      <c r="L93" s="2"/>
+      <c r="M93" s="2"/>
+      <c r="N93" s="2"/>
+      <c r="O93" s="2"/>
+      <c r="P93" s="2"/>
+      <c r="Q93" s="2"/>
+      <c r="R93" s="2"/>
+      <c r="S93" s="2"/>
+      <c r="T93" s="2"/>
+      <c r="U93" s="2"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="2"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="2"/>
+      <c r="H94" s="2"/>
+      <c r="I94" s="2"/>
+      <c r="J94" s="2"/>
+      <c r="K94" s="2"/>
+      <c r="L94" s="2"/>
+      <c r="M94" s="2"/>
+      <c r="N94" s="2"/>
+      <c r="O94" s="2"/>
+      <c r="P94" s="2"/>
+      <c r="Q94" s="2"/>
+      <c r="R94" s="2"/>
+      <c r="S94" s="2"/>
+      <c r="T94" s="2"/>
+      <c r="U94" s="2"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="2"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="2"/>
+      <c r="H95" s="2"/>
+      <c r="I95" s="2"/>
+      <c r="J95" s="2"/>
+      <c r="K95" s="2"/>
+      <c r="L95" s="2"/>
+      <c r="M95" s="2"/>
+      <c r="N95" s="2"/>
+      <c r="O95" s="2"/>
+      <c r="P95" s="2"/>
+      <c r="Q95" s="2"/>
+      <c r="R95" s="2"/>
+      <c r="S95" s="2"/>
+      <c r="T95" s="2"/>
+      <c r="U95" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" location="dfn-contrast-ratio" ref="E26"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>